<commit_message>
all CASE CE and HE recalculated
</commit_message>
<xml_diff>
--- a/ASHRAE_140/HEATING_TEST/Std140_HE_Results.xlsx
+++ b/ASHRAE_140/HEATING_TEST/Std140_HE_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10518"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfc/Documents/OpenSimula/ASHRAE_140/HEATING_TEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF90833A-8DBB-0C4E-AC2B-9B144C6B50B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762FC447-9B6A-1E41-AD9E-424619E9ADE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45380" yWindow="2360" windowWidth="38400" windowHeight="21100" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44800" yWindow="2300" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="17" r:id="rId1"/>
@@ -1267,7 +1267,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1437,6 +1437,12 @@
       <color rgb="FF3B3B3B"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3B3B3B"/>
+      <name val="Menlo"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2409,7 +2415,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="370">
+  <cellXfs count="371">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3327,11 +3333,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="73" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="74" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3357,6 +3369,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="67" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -3366,19 +3384,8 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="73" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="74" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="11" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3992,25 +3999,25 @@
                   <c:v>31.154426381399801</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10360804996534401</c:v>
+                  <c:v>0.103608049965337</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>31.154426381399801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.686409068948901</c:v>
+                  <c:v>29.6864363286189</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>30.543555275882099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.686409068948901</c:v>
+                  <c:v>29.6864363286189</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>42.0772599771784</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39.849500586513102</c:v>
+                  <c:v>39.849504467827103</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>34.621779017509198</c:v>
@@ -4829,25 +4836,25 @@
                   <c:v>38.344457083638801</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89564863548367402</c:v>
+                  <c:v>0.89564863548366602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.968343464704098</c:v>
+                  <c:v>38.968343464703999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.057595333156698</c:v>
+                  <c:v>37.057625829205499</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>38.192690862959402</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.057595333156698</c:v>
+                  <c:v>37.057625829205499</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>52.452936144981997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49.593084849220901</c:v>
+                  <c:v>49.593087839326898</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>43.354476382326702</c:v>
@@ -5666,25 +5673,25 @@
                   <c:v>1.2976654579420699E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0310829390150299E-6</c:v>
+                  <c:v>3.0310829390149998E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.31877922165042E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.25411506840063E-4</c:v>
+                  <c:v>1.2541161004577301E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.29252933665527E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.25411506840063E-4</c:v>
+                  <c:v>1.2541161004577301E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.7751291472067199E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6783451392009399E-4</c:v>
+                  <c:v>1.6783452403930699E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.4672161435431099E-4</c:v>
@@ -6487,13 +6494,13 @@
                   <c:v>169.745292724264</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>473.17510592572899</c:v>
+                  <c:v>473.17513981022802</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>291.40520080545502</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>275.51713805122699</c:v>
+                  <c:v>275.517154662927</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>481.71640424807498</c:v>
@@ -8575,7 +8582,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Chart11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -13949,8 +13956,8 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -13980,13 +13987,13 @@
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="365" t="s">
+      <c r="F2" s="353" t="s">
         <v>303</v>
       </c>
-      <c r="G2" s="366"/>
-      <c r="H2" s="366"/>
-      <c r="I2" s="366"/>
-      <c r="J2" s="367"/>
+      <c r="G2" s="354"/>
+      <c r="H2" s="354"/>
+      <c r="I2" s="354"/>
+      <c r="J2" s="355"/>
       <c r="K2" s="102" t="s">
         <v>52</v>
       </c>
@@ -14017,7 +14024,7 @@
       <c r="G4" s="326"/>
       <c r="H4" s="326"/>
       <c r="I4" s="326"/>
-      <c r="J4" s="368" t="s">
+      <c r="J4" s="352" t="s">
         <v>304</v>
       </c>
       <c r="K4" s="102" t="s">
@@ -14066,13 +14073,13 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="365" t="s">
+      <c r="F7" s="353" t="s">
         <v>305</v>
       </c>
-      <c r="G7" s="366"/>
-      <c r="H7" s="366"/>
-      <c r="I7" s="366"/>
-      <c r="J7" s="367"/>
+      <c r="G7" s="354"/>
+      <c r="H7" s="354"/>
+      <c r="I7" s="354"/>
+      <c r="J7" s="355"/>
       <c r="K7" s="103"/>
     </row>
     <row r="8" spans="1:14" ht="16">
@@ -14087,13 +14094,13 @@
       <c r="G8" s="326"/>
       <c r="H8" s="326"/>
       <c r="I8" s="326"/>
-      <c r="J8" s="365" t="s">
+      <c r="J8" s="353" t="s">
         <v>306</v>
       </c>
-      <c r="K8" s="366"/>
-      <c r="L8" s="366"/>
-      <c r="M8" s="366"/>
-      <c r="N8" s="367"/>
+      <c r="K8" s="354"/>
+      <c r="L8" s="354"/>
+      <c r="M8" s="354"/>
+      <c r="N8" s="355"/>
     </row>
     <row r="9" spans="1:14" ht="16">
       <c r="A9" s="1" t="s">
@@ -14247,7 +14254,7 @@
       <c r="A20" s="240" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="351">
+      <c r="B20" s="369">
         <v>77.730653878551493</v>
       </c>
     </row>
@@ -14255,7 +14262,7 @@
       <c r="A21" s="240" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="351">
+      <c r="B21" s="369">
         <v>77.730653878551493</v>
       </c>
     </row>
@@ -14263,7 +14270,7 @@
       <c r="A22" s="240" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="351">
+      <c r="B22" s="369">
         <v>31.154426381399801</v>
       </c>
     </row>
@@ -14271,15 +14278,15 @@
       <c r="A23" s="240" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="351">
-        <v>0.10360804996534401</v>
+      <c r="B23" s="369">
+        <v>0.103608049965337</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="16">
       <c r="A24" s="240" t="s">
         <v>113</v>
       </c>
-      <c r="B24" s="351">
+      <c r="B24" s="369">
         <v>31.154426381399801</v>
       </c>
     </row>
@@ -14287,15 +14294,15 @@
       <c r="A25" s="240" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="351">
-        <v>29.686409068948901</v>
+      <c r="B25" s="369">
+        <v>29.6864363286189</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="16">
       <c r="A26" s="240" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="351">
+      <c r="B26" s="369">
         <v>30.543555275882099</v>
       </c>
     </row>
@@ -14303,15 +14310,15 @@
       <c r="A27" s="240" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="351">
-        <v>29.686409068948901</v>
+      <c r="B27" s="369">
+        <v>29.6864363286189</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="16">
       <c r="A28" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="351">
+      <c r="B28" s="369">
         <v>42.0772599771784</v>
       </c>
     </row>
@@ -14319,8 +14326,8 @@
       <c r="A29" s="240" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="351">
-        <v>39.849500586513102</v>
+      <c r="B29" s="369">
+        <v>39.849504467827103</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="16">
@@ -14390,7 +14397,7 @@
       <c r="A36" s="240" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="351">
+      <c r="B36" s="369">
         <v>77.728737653539696</v>
       </c>
     </row>
@@ -14398,7 +14405,7 @@
       <c r="A37" s="240" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="351">
+      <c r="B37" s="369">
         <v>97.160922066924599</v>
       </c>
     </row>
@@ -14406,7 +14413,7 @@
       <c r="A38" s="240" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="351">
+      <c r="B38" s="369">
         <v>38.344457083638801</v>
       </c>
     </row>
@@ -14414,31 +14421,31 @@
       <c r="A39" s="240" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="351">
-        <v>0.89564863548367402</v>
+      <c r="B39" s="369">
+        <v>0.89564863548366602</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="16">
       <c r="A40" s="240" t="s">
         <v>113</v>
       </c>
-      <c r="B40" s="351">
-        <v>38.968343464704098</v>
+      <c r="B40" s="369">
+        <v>38.968343464703999</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16">
       <c r="A41" s="240" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="351">
-        <v>37.057595333156698</v>
+      <c r="B41" s="369">
+        <v>37.057625829205499</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="16">
       <c r="A42" s="240" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="351">
+      <c r="B42" s="369">
         <v>38.192690862959402</v>
       </c>
     </row>
@@ -14446,15 +14453,15 @@
       <c r="A43" s="240" t="s">
         <v>116</v>
       </c>
-      <c r="B43" s="351">
-        <v>37.057595333156698</v>
+      <c r="B43" s="369">
+        <v>37.057625829205499</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="16">
       <c r="A44" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="351">
+      <c r="B44" s="369">
         <v>52.452936144981997</v>
       </c>
     </row>
@@ -14462,8 +14469,8 @@
       <c r="A45" s="240" t="s">
         <v>118</v>
       </c>
-      <c r="B45" s="351">
-        <v>49.593084849220901</v>
+      <c r="B45" s="369">
+        <v>49.593087839326898</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="16">
@@ -14526,7 +14533,7 @@
       <c r="A52" s="240" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="351">
+      <c r="B52" s="369">
         <v>2.6305209569775999E-4</v>
       </c>
     </row>
@@ -14534,7 +14541,7 @@
       <c r="A53" s="240" t="s">
         <v>110</v>
       </c>
-      <c r="B53" s="351">
+      <c r="B53" s="369">
         <v>3.2881511962219999E-4</v>
       </c>
     </row>
@@ -14542,7 +14549,7 @@
       <c r="A54" s="240" t="s">
         <v>111</v>
       </c>
-      <c r="B54" s="351">
+      <c r="B54" s="369">
         <v>1.2976654579420699E-4</v>
       </c>
     </row>
@@ -14550,15 +14557,15 @@
       <c r="A55" s="240" t="s">
         <v>112</v>
       </c>
-      <c r="B55" s="369">
-        <v>3.0310829390150299E-6</v>
+      <c r="B55" s="370">
+        <v>3.0310829390149998E-6</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="16">
       <c r="A56" s="240" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="351">
+      <c r="B56" s="369">
         <v>1.31877922165042E-4</v>
       </c>
     </row>
@@ -14566,15 +14573,15 @@
       <c r="A57" s="240" t="s">
         <v>114</v>
       </c>
-      <c r="B57" s="351">
-        <v>1.25411506840063E-4</v>
+      <c r="B57" s="369">
+        <v>1.2541161004577301E-4</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="16">
       <c r="A58" s="240" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="351">
+      <c r="B58" s="369">
         <v>1.29252933665527E-4</v>
       </c>
     </row>
@@ -14582,15 +14589,15 @@
       <c r="A59" s="240" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="351">
-        <v>1.25411506840063E-4</v>
+      <c r="B59" s="369">
+        <v>1.2541161004577301E-4</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="16">
       <c r="A60" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="351">
+      <c r="B60" s="369">
         <v>1.7751291472067199E-4</v>
       </c>
     </row>
@@ -14598,8 +14605,8 @@
       <c r="A61" s="240" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="351">
-        <v>1.6783451392009399E-4</v>
+      <c r="B61" s="369">
+        <v>1.6783452403930699E-4</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="16">
@@ -14663,7 +14670,7 @@
       <c r="A68" s="240" t="s">
         <v>114</v>
       </c>
-      <c r="B68" s="351">
+      <c r="B68" s="369">
         <v>432</v>
       </c>
     </row>
@@ -14671,7 +14678,7 @@
       <c r="A69" s="240" t="s">
         <v>115</v>
       </c>
-      <c r="B69" s="351">
+      <c r="B69" s="369">
         <v>169.745292724264</v>
       </c>
     </row>
@@ -14679,15 +14686,15 @@
       <c r="A70" s="240" t="s">
         <v>116</v>
       </c>
-      <c r="B70" s="351">
-        <v>473.17510592572899</v>
+      <c r="B70" s="369">
+        <v>473.17513981022802</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="16">
       <c r="A71" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="B71" s="351">
+      <c r="B71" s="369">
         <v>291.40520080545502</v>
       </c>
     </row>
@@ -14695,8 +14702,8 @@
       <c r="A72" s="240" t="s">
         <v>118</v>
       </c>
-      <c r="B72" s="351">
-        <v>275.51713805122699</v>
+      <c r="B72" s="369">
+        <v>275.517154662927</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="16">
@@ -14739,7 +14746,7 @@
       <c r="A79" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="B79" s="351">
+      <c r="B79" s="369">
         <v>20</v>
       </c>
     </row>
@@ -14747,7 +14754,7 @@
       <c r="A80" s="240" t="s">
         <v>118</v>
       </c>
-      <c r="B80" s="351">
+      <c r="B80" s="369">
         <v>18.5416666666666</v>
       </c>
     </row>
@@ -14818,7 +14825,7 @@
       <c r="A87" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="B87" s="351">
+      <c r="B87" s="369">
         <v>20</v>
       </c>
       <c r="C87" s="9"/>
@@ -14828,7 +14835,7 @@
       <c r="A88" s="240" t="s">
         <v>118</v>
       </c>
-      <c r="B88" s="351">
+      <c r="B88" s="369">
         <v>20</v>
       </c>
       <c r="C88" s="9"/>
@@ -14903,7 +14910,7 @@
       <c r="A95" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="B95" s="351">
+      <c r="B95" s="369">
         <v>19.999999999999901</v>
       </c>
       <c r="C95" s="9"/>
@@ -14913,7 +14920,7 @@
       <c r="A96" s="240" t="s">
         <v>118</v>
       </c>
-      <c r="B96" s="351">
+      <c r="B96" s="369">
         <v>14.999999999999901</v>
       </c>
       <c r="C96" s="9"/>
@@ -15739,45 +15746,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A1" s="352" t="str">
+      <c r="A1" s="364" t="str">
         <f>IF('Title Page'!$B$21="Example",'Title Page'!$B$30,"ASHRAE Standard 140-2023 Section 10 - HVAC Equipment Performance Tests HE100-HE230")</f>
         <v>ASHRAE Standard 140-2023, Informative Annex B16, Section B16.6</v>
       </c>
-      <c r="B1" s="352"/>
-      <c r="C1" s="352"/>
-      <c r="D1" s="352"/>
-      <c r="E1" s="352"/>
-      <c r="F1" s="352"/>
+      <c r="B1" s="364"/>
+      <c r="C1" s="364"/>
+      <c r="D1" s="364"/>
+      <c r="E1" s="364"/>
+      <c r="F1" s="364"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A2" s="352" t="str">
+      <c r="A2" s="364" t="str">
         <f>'Title Page'!$B$32</f>
         <v>Example Results for Section 10 - HVAC Equipment Performance Tests HE100 through HE230</v>
       </c>
-      <c r="B2" s="352"/>
-      <c r="C2" s="352"/>
-      <c r="D2" s="352"/>
-      <c r="E2" s="352"/>
-      <c r="F2" s="352"/>
+      <c r="B2" s="364"/>
+      <c r="C2" s="364"/>
+      <c r="D2" s="364"/>
+      <c r="E2" s="364"/>
+      <c r="F2" s="364"/>
     </row>
     <row r="3" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A3" s="352" t="str">
+      <c r="A3" s="364" t="str">
         <f>'Title Page'!$B$34</f>
         <v/>
       </c>
-      <c r="B3" s="352"/>
-      <c r="C3" s="352"/>
-      <c r="D3" s="352"/>
-      <c r="E3" s="352"/>
-      <c r="F3" s="352"/>
+      <c r="B3" s="364"/>
+      <c r="C3" s="364"/>
+      <c r="D3" s="364"/>
+      <c r="E3" s="364"/>
+      <c r="F3" s="364"/>
     </row>
     <row r="5" spans="1:6" ht="13.5" customHeight="1">
-      <c r="B5" s="353" t="s">
+      <c r="B5" s="365" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="353"/>
-      <c r="D5" s="353"/>
-      <c r="E5" s="353"/>
+      <c r="C5" s="365"/>
+      <c r="D5" s="365"/>
+      <c r="E5" s="365"/>
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" thickBot="1">
       <c r="B6" s="276"/>
@@ -15904,12 +15911,12 @@
       <c r="E15" s="276"/>
     </row>
     <row r="20" spans="1:5" ht="17.25" customHeight="1">
-      <c r="B20" s="353" t="s">
+      <c r="B20" s="365" t="s">
         <v>217</v>
       </c>
-      <c r="C20" s="353"/>
-      <c r="D20" s="353"/>
-      <c r="E20" s="353"/>
+      <c r="C20" s="365"/>
+      <c r="D20" s="365"/>
+      <c r="E20" s="365"/>
     </row>
     <row r="21" spans="1:5" ht="13.5" customHeight="1" thickBot="1">
       <c r="A21" t="str">
@@ -15928,10 +15935,10 @@
       <c r="C22" s="301" t="s">
         <v>201</v>
       </c>
-      <c r="D22" s="358" t="s">
+      <c r="D22" s="360" t="s">
         <v>202</v>
       </c>
-      <c r="E22" s="359"/>
+      <c r="E22" s="361"/>
     </row>
     <row r="23" spans="1:5" ht="13.5" customHeight="1" thickTop="1">
       <c r="B23" s="294" t="s">
@@ -15940,10 +15947,10 @@
       <c r="C23" s="295" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="360" t="s">
+      <c r="D23" s="362" t="s">
         <v>219</v>
       </c>
-      <c r="E23" s="361"/>
+      <c r="E23" s="363"/>
     </row>
     <row r="24" spans="1:5" ht="13.5" customHeight="1">
       <c r="B24" s="296" t="s">
@@ -15952,10 +15959,10 @@
       <c r="C24" s="304" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="354" t="s">
+      <c r="D24" s="356" t="s">
         <v>220</v>
       </c>
-      <c r="E24" s="355"/>
+      <c r="E24" s="357"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="B25" s="296" t="s">
@@ -15964,10 +15971,10 @@
       <c r="C25" s="304" t="s">
         <v>212</v>
       </c>
-      <c r="D25" s="354" t="s">
+      <c r="D25" s="356" t="s">
         <v>221</v>
       </c>
-      <c r="E25" s="355"/>
+      <c r="E25" s="357"/>
     </row>
     <row r="26" spans="1:5" ht="13.5" customHeight="1">
       <c r="B26" s="296" t="s">
@@ -15976,10 +15983,10 @@
       <c r="C26" s="304" t="s">
         <v>213</v>
       </c>
-      <c r="D26" s="354" t="s">
+      <c r="D26" s="356" t="s">
         <v>222</v>
       </c>
-      <c r="E26" s="355"/>
+      <c r="E26" s="357"/>
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="B27" s="296" t="s">
@@ -15988,10 +15995,10 @@
       <c r="C27" s="304" t="s">
         <v>214</v>
       </c>
-      <c r="D27" s="354" t="s">
+      <c r="D27" s="356" t="s">
         <v>223</v>
       </c>
-      <c r="E27" s="355"/>
+      <c r="E27" s="357"/>
     </row>
     <row r="28" spans="1:5" ht="13.5" customHeight="1">
       <c r="B28" s="296" t="s">
@@ -16000,10 +16007,10 @@
       <c r="C28" s="304" t="s">
         <v>215</v>
       </c>
-      <c r="D28" s="354" t="s">
+      <c r="D28" s="356" t="s">
         <v>225</v>
       </c>
-      <c r="E28" s="355"/>
+      <c r="E28" s="357"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1" thickBot="1">
       <c r="B29" s="307" t="s">
@@ -16012,14 +16019,19 @@
       <c r="C29" s="308" t="s">
         <v>216</v>
       </c>
-      <c r="D29" s="356" t="s">
+      <c r="D29" s="358" t="s">
         <v>224</v>
       </c>
-      <c r="E29" s="357"/>
+      <c r="E29" s="359"/>
     </row>
     <row r="30" spans="1:5" ht="13.5" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D22:E22"/>
@@ -16028,11 +16040,6 @@
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -16068,54 +16075,54 @@
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1">
       <c r="A1" s="103"/>
-      <c r="B1" s="352" t="str">
+      <c r="B1" s="364" t="str">
         <f>'Title Page'!$B$30</f>
         <v>ASHRAE Standard 140-2023, Informative Annex B16, Section B16.6</v>
       </c>
-      <c r="C1" s="352"/>
-      <c r="D1" s="352"/>
-      <c r="E1" s="352"/>
-      <c r="F1" s="352"/>
-      <c r="G1" s="352"/>
-      <c r="H1" s="352"/>
-      <c r="I1" s="352"/>
-      <c r="J1" s="352"/>
-      <c r="K1" s="352"/>
-      <c r="L1" s="352"/>
+      <c r="C1" s="364"/>
+      <c r="D1" s="364"/>
+      <c r="E1" s="364"/>
+      <c r="F1" s="364"/>
+      <c r="G1" s="364"/>
+      <c r="H1" s="364"/>
+      <c r="I1" s="364"/>
+      <c r="J1" s="364"/>
+      <c r="K1" s="364"/>
+      <c r="L1" s="364"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
       <c r="A2" s="103"/>
-      <c r="B2" s="352" t="str">
+      <c r="B2" s="364" t="str">
         <f>'Title Page'!$B$32</f>
         <v>Example Results for Section 10 - HVAC Equipment Performance Tests HE100 through HE230</v>
       </c>
-      <c r="C2" s="352"/>
-      <c r="D2" s="352"/>
-      <c r="E2" s="352"/>
-      <c r="F2" s="352"/>
-      <c r="G2" s="352"/>
-      <c r="H2" s="352"/>
-      <c r="I2" s="352"/>
-      <c r="J2" s="352"/>
-      <c r="K2" s="352"/>
-      <c r="L2" s="352"/>
+      <c r="C2" s="364"/>
+      <c r="D2" s="364"/>
+      <c r="E2" s="364"/>
+      <c r="F2" s="364"/>
+      <c r="G2" s="364"/>
+      <c r="H2" s="364"/>
+      <c r="I2" s="364"/>
+      <c r="J2" s="364"/>
+      <c r="K2" s="364"/>
+      <c r="L2" s="364"/>
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1">
       <c r="A3" s="103"/>
-      <c r="B3" s="352" t="str">
+      <c r="B3" s="364" t="str">
         <f>'Title Page'!$B$34</f>
         <v/>
       </c>
-      <c r="C3" s="352"/>
-      <c r="D3" s="352"/>
-      <c r="E3" s="352"/>
-      <c r="F3" s="352"/>
-      <c r="G3" s="352"/>
-      <c r="H3" s="352"/>
-      <c r="I3" s="352"/>
-      <c r="J3" s="352"/>
-      <c r="K3" s="352"/>
-      <c r="L3" s="352"/>
+      <c r="C3" s="364"/>
+      <c r="D3" s="364"/>
+      <c r="E3" s="364"/>
+      <c r="F3" s="364"/>
+      <c r="G3" s="364"/>
+      <c r="H3" s="364"/>
+      <c r="I3" s="364"/>
+      <c r="J3" s="364"/>
+      <c r="K3" s="364"/>
+      <c r="L3" s="364"/>
     </row>
     <row r="4" spans="1:12" ht="16.5" customHeight="1">
       <c r="A4" s="103"/>
@@ -16154,12 +16161,12 @@
       <c r="C8" s="166"/>
       <c r="D8" s="167"/>
       <c r="E8" s="168"/>
-      <c r="F8" s="362" t="s">
+      <c r="F8" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="363"/>
-      <c r="H8" s="363"/>
-      <c r="I8" s="364"/>
+      <c r="G8" s="367"/>
+      <c r="H8" s="367"/>
+      <c r="I8" s="368"/>
       <c r="K8" s="155"/>
       <c r="L8" s="343"/>
     </row>
@@ -16379,7 +16386,7 @@
       </c>
       <c r="K14" s="158">
         <f>A!E33</f>
-        <v>0.10360804996534401</v>
+        <v>0.103608049965337</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="16">
@@ -16457,7 +16464,7 @@
       </c>
       <c r="K16" s="158">
         <f>A!E35</f>
-        <v>29.686409068948901</v>
+        <v>29.6864363286189</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16">
@@ -16535,7 +16542,7 @@
       </c>
       <c r="K18" s="237">
         <f>A!E37</f>
-        <v>29.686409068948901</v>
+        <v>29.6864363286189</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="16">
@@ -16690,7 +16697,7 @@
       </c>
       <c r="K22" s="158">
         <f>A!E39</f>
-        <v>39.849500586513102</v>
+        <v>39.849504467827103</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="17" thickBot="1">
@@ -16786,12 +16793,12 @@
       <c r="C27" s="166"/>
       <c r="D27" s="167"/>
       <c r="E27" s="168"/>
-      <c r="F27" s="362" t="s">
+      <c r="F27" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="363"/>
-      <c r="H27" s="363"/>
-      <c r="I27" s="364"/>
+      <c r="G27" s="367"/>
+      <c r="H27" s="367"/>
+      <c r="I27" s="368"/>
       <c r="J27" s="177"/>
       <c r="K27" s="155"/>
     </row>
@@ -17015,7 +17022,7 @@
       </c>
       <c r="K33" s="158">
         <f>A!I33</f>
-        <v>0.89564863548367402</v>
+        <v>0.89564863548366602</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="16">
@@ -17055,7 +17062,7 @@
       </c>
       <c r="K34" s="158">
         <f>A!I34</f>
-        <v>38.968343464704098</v>
+        <v>38.968343464703999</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="16">
@@ -17095,7 +17102,7 @@
       </c>
       <c r="K35" s="158">
         <f>A!I35</f>
-        <v>37.057595333156698</v>
+        <v>37.057625829205499</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="16">
@@ -17175,7 +17182,7 @@
       </c>
       <c r="K37" s="237">
         <f>A!I37</f>
-        <v>37.057595333156698</v>
+        <v>37.057625829205499</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16">
@@ -17325,7 +17332,7 @@
       </c>
       <c r="K41" s="158">
         <f>A!I39</f>
-        <v>49.593084849220901</v>
+        <v>49.593087839326898</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="17" thickBot="1">
@@ -17421,12 +17428,12 @@
       <c r="C46" s="166"/>
       <c r="D46" s="167"/>
       <c r="E46" s="168"/>
-      <c r="F46" s="362" t="s">
+      <c r="F46" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="G46" s="363"/>
-      <c r="H46" s="363"/>
-      <c r="I46" s="364"/>
+      <c r="G46" s="367"/>
+      <c r="H46" s="367"/>
+      <c r="I46" s="368"/>
       <c r="J46" s="177"/>
       <c r="K46" s="155"/>
     </row>
@@ -17646,7 +17653,7 @@
       </c>
       <c r="K52" s="163">
         <f>A!M33</f>
-        <v>3.0310829390150299E-6</v>
+        <v>3.0310829390149998E-6</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16">
@@ -17724,7 +17731,7 @@
       </c>
       <c r="K54" s="163">
         <f>A!M35</f>
-        <v>1.25411506840063E-4</v>
+        <v>1.2541161004577301E-4</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16">
@@ -17802,7 +17809,7 @@
       </c>
       <c r="K56" s="246">
         <f>A!M37</f>
-        <v>1.25411506840063E-4</v>
+        <v>1.2541161004577301E-4</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="16">
@@ -17952,7 +17959,7 @@
       </c>
       <c r="K60" s="163">
         <f>A!M39</f>
-        <v>1.6783451392009399E-4</v>
+        <v>1.6783452403930699E-4</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="17" thickBot="1">
@@ -18048,12 +18055,12 @@
       <c r="C65" s="166"/>
       <c r="D65" s="167"/>
       <c r="E65" s="168"/>
-      <c r="F65" s="362" t="s">
+      <c r="F65" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="363"/>
-      <c r="H65" s="363"/>
-      <c r="I65" s="364"/>
+      <c r="G65" s="367"/>
+      <c r="H65" s="367"/>
+      <c r="I65" s="368"/>
       <c r="J65" s="177"/>
       <c r="K65" s="155"/>
     </row>
@@ -18235,7 +18242,7 @@
       </c>
       <c r="K70" s="250">
         <f>A!E49</f>
-        <v>473.17510592572899</v>
+        <v>473.17513981022802</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="16">
@@ -18385,7 +18392,7 @@
       </c>
       <c r="K74" s="190">
         <f>A!E51</f>
-        <v>275.51713805122699</v>
+        <v>275.517154662927</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="17" thickBot="1">
@@ -18482,12 +18489,12 @@
       <c r="C79" s="166"/>
       <c r="D79" s="167"/>
       <c r="E79" s="168"/>
-      <c r="F79" s="362" t="s">
+      <c r="F79" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="G79" s="363"/>
-      <c r="H79" s="363"/>
-      <c r="I79" s="363"/>
+      <c r="G79" s="367"/>
+      <c r="H79" s="367"/>
+      <c r="I79" s="367"/>
       <c r="J79" s="155"/>
       <c r="L79" s="133"/>
     </row>
@@ -18723,12 +18730,12 @@
       <c r="C88" s="166"/>
       <c r="D88" s="167"/>
       <c r="E88" s="168"/>
-      <c r="F88" s="362" t="s">
+      <c r="F88" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="G88" s="363"/>
-      <c r="H88" s="363"/>
-      <c r="I88" s="364"/>
+      <c r="G88" s="367"/>
+      <c r="H88" s="367"/>
+      <c r="I88" s="368"/>
       <c r="J88" s="155"/>
       <c r="K88" s="133"/>
       <c r="L88" s="133"/>
@@ -18971,12 +18978,12 @@
       <c r="C97" s="166"/>
       <c r="D97" s="167"/>
       <c r="E97" s="168"/>
-      <c r="F97" s="362" t="s">
+      <c r="F97" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="G97" s="363"/>
-      <c r="H97" s="363"/>
-      <c r="I97" s="364"/>
+      <c r="G97" s="367"/>
+      <c r="H97" s="367"/>
+      <c r="I97" s="368"/>
       <c r="J97" s="155"/>
       <c r="K97" s="133"/>
       <c r="L97" s="133"/>
@@ -23942,16 +23949,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F88:I88"/>
     <mergeCell ref="F97:I97"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="F46:I46"/>
     <mergeCell ref="F65:I65"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F88:I88"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="1" right="0.5" top="0.3" bottom="0.5" header="0.5" footer="0.5"/>
@@ -24698,7 +24705,7 @@
       </c>
       <c r="E33" s="55">
         <f>IF(ISNUMBER(YourData!$B23),YourData!$B23,"")</f>
-        <v>0.10360804996534401</v>
+        <v>0.103608049965337</v>
       </c>
       <c r="F33" s="65">
         <f>IF(ISNUMBER('ESP-HOT'!$B39),'ESP-HOT'!$B39,"")</f>
@@ -24714,7 +24721,7 @@
       </c>
       <c r="I33" s="55">
         <f>IF(ISNUMBER(YourData!$B39),YourData!$B39,"")</f>
-        <v>0.89564863548367402</v>
+        <v>0.89564863548366602</v>
       </c>
       <c r="J33" s="225">
         <f>IF(ISNUMBER('ESP-HOT'!$B55),'ESP-HOT'!$B55,"")</f>
@@ -24730,7 +24737,7 @@
       </c>
       <c r="M33" s="98">
         <f>IF(ISNUMBER(YourData!$B55),YourData!$B55,"")</f>
-        <v>3.0310829390150299E-6</v>
+        <v>3.0310829390149998E-6</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -24768,7 +24775,7 @@
       </c>
       <c r="I34" s="55">
         <f>IF(ISNUMBER(YourData!$B40),YourData!$B40,"")</f>
-        <v>38.968343464704098</v>
+        <v>38.968343464703999</v>
       </c>
       <c r="J34" s="225">
         <f>IF(ISNUMBER('ESP-HOT'!$B56),'ESP-HOT'!$B56,"")</f>
@@ -24806,7 +24813,7 @@
       </c>
       <c r="E35" s="55">
         <f>IF(ISNUMBER(YourData!$B25),YourData!$B25,"")</f>
-        <v>29.686409068948901</v>
+        <v>29.6864363286189</v>
       </c>
       <c r="F35" s="65">
         <f>IF(ISNUMBER('ESP-HOT'!$B41),'ESP-HOT'!$B41,"")</f>
@@ -24822,7 +24829,7 @@
       </c>
       <c r="I35" s="55">
         <f>IF(ISNUMBER(YourData!$B41),YourData!$B41,"")</f>
-        <v>37.057595333156698</v>
+        <v>37.057625829205499</v>
       </c>
       <c r="J35" s="225">
         <f>IF(ISNUMBER('ESP-HOT'!$B57),'ESP-HOT'!$B57,"")</f>
@@ -24838,7 +24845,7 @@
       </c>
       <c r="M35" s="98">
         <f>IF(ISNUMBER(YourData!$B57),YourData!$B57,"")</f>
-        <v>1.25411506840063E-4</v>
+        <v>1.2541161004577301E-4</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -24914,7 +24921,7 @@
       </c>
       <c r="E37" s="55">
         <f>IF(ISNUMBER(YourData!$B27),YourData!$B27,"")</f>
-        <v>29.686409068948901</v>
+        <v>29.6864363286189</v>
       </c>
       <c r="F37" s="65">
         <f>IF(ISNUMBER('ESP-HOT'!$B43),'ESP-HOT'!$B43,"")</f>
@@ -24930,7 +24937,7 @@
       </c>
       <c r="I37" s="55">
         <f>IF(ISNUMBER(YourData!$B43),YourData!$B43,"")</f>
-        <v>37.057595333156698</v>
+        <v>37.057625829205499</v>
       </c>
       <c r="J37" s="225">
         <f>IF(ISNUMBER('ESP-HOT'!$B59),'ESP-HOT'!$B59,"")</f>
@@ -24946,7 +24953,7 @@
       </c>
       <c r="M37" s="98">
         <f>IF(ISNUMBER(YourData!$B59),YourData!$B59,"")</f>
-        <v>1.25411506840063E-4</v>
+        <v>1.2541161004577301E-4</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -25022,7 +25029,7 @@
       </c>
       <c r="E39" s="55">
         <f>IF(ISNUMBER(YourData!$B29),YourData!$B29,"")</f>
-        <v>39.849500586513102</v>
+        <v>39.849504467827103</v>
       </c>
       <c r="F39" s="65">
         <f>IF(ISNUMBER('ESP-HOT'!$B45),'ESP-HOT'!$B45,"")</f>
@@ -25038,7 +25045,7 @@
       </c>
       <c r="I39" s="55">
         <f>IF(ISNUMBER(YourData!$B45),YourData!$B45,"")</f>
-        <v>49.593084849220901</v>
+        <v>49.593087839326898</v>
       </c>
       <c r="J39" s="225">
         <f>IF(ISNUMBER('ESP-HOT'!$B61),'ESP-HOT'!$B61,"")</f>
@@ -25054,7 +25061,7 @@
       </c>
       <c r="M39" s="98">
         <f>IF(ISNUMBER(YourData!$B61),YourData!$B61,"")</f>
-        <v>1.6783451392009399E-4</v>
+        <v>1.6783452403930699E-4</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="14" thickBot="1">
@@ -25235,7 +25242,7 @@
       </c>
       <c r="E49" s="220">
         <f>IF(ISNUMBER(YourData!$B70),YourData!$B70,"")</f>
-        <v>473.17510592572899</v>
+        <v>473.17513981022802</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -25279,7 +25286,7 @@
       </c>
       <c r="E51" s="220">
         <f>IF(ISNUMBER(YourData!$B72),YourData!$B72,"")</f>
-        <v>275.51713805122699</v>
+        <v>275.517154662927</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="14" thickBot="1">
@@ -25680,11 +25687,11 @@
       <c r="B6" s="166"/>
       <c r="C6" s="167"/>
       <c r="D6" s="168"/>
-      <c r="E6" s="362" t="s">
+      <c r="E6" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="363"/>
-      <c r="G6" s="364"/>
+      <c r="F6" s="367"/>
+      <c r="G6" s="368"/>
       <c r="H6" s="169" t="s">
         <v>97</v>
       </c>
@@ -25878,7 +25885,7 @@
       </c>
       <c r="I12" s="158">
         <f>A!E33</f>
-        <v>0.10360804996534401</v>
+        <v>0.103608049965337</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -25952,7 +25959,7 @@
       </c>
       <c r="I14" s="158">
         <f>A!E35</f>
-        <v>29.686409068948901</v>
+        <v>29.6864363286189</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -26026,7 +26033,7 @@
       </c>
       <c r="I16" s="237">
         <f>A!E37</f>
-        <v>29.686409068948901</v>
+        <v>29.6864363286189</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -26100,7 +26107,7 @@
       </c>
       <c r="I18" s="158">
         <f>A!E39</f>
-        <v>39.849500586513102</v>
+        <v>39.849504467827103</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14" thickBot="1">
@@ -26171,11 +26178,11 @@
       <c r="B22" s="166"/>
       <c r="C22" s="167"/>
       <c r="D22" s="168"/>
-      <c r="E22" s="362" t="s">
+      <c r="E22" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="F22" s="363"/>
-      <c r="G22" s="364"/>
+      <c r="F22" s="367"/>
+      <c r="G22" s="368"/>
       <c r="H22" s="169" t="s">
         <v>97</v>
       </c>
@@ -26372,7 +26379,7 @@
       </c>
       <c r="I28" s="158">
         <f>A!I33</f>
-        <v>0.89564863548367402</v>
+        <v>0.89564863548366602</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -26410,7 +26417,7 @@
       </c>
       <c r="I29" s="158">
         <f>A!I34</f>
-        <v>38.968343464704098</v>
+        <v>38.968343464703999</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -26448,7 +26455,7 @@
       </c>
       <c r="I30" s="158">
         <f>A!I35</f>
-        <v>37.057595333156698</v>
+        <v>37.057625829205499</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -26524,7 +26531,7 @@
       </c>
       <c r="I32" s="237">
         <f>A!I37</f>
-        <v>37.057595333156698</v>
+        <v>37.057625829205499</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -26598,7 +26605,7 @@
       </c>
       <c r="I34" s="158">
         <f>A!I39</f>
-        <v>49.593084849220901</v>
+        <v>49.593087839326898</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="14" thickBot="1">
@@ -26669,11 +26676,11 @@
       <c r="B38" s="166"/>
       <c r="C38" s="167"/>
       <c r="D38" s="168"/>
-      <c r="E38" s="362" t="s">
+      <c r="E38" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="F38" s="363"/>
-      <c r="G38" s="364"/>
+      <c r="F38" s="367"/>
+      <c r="G38" s="368"/>
       <c r="H38" s="169" t="s">
         <v>97</v>
       </c>
@@ -26866,7 +26873,7 @@
       </c>
       <c r="I44" s="163">
         <f>A!M33</f>
-        <v>3.0310829390150299E-6</v>
+        <v>3.0310829390149998E-6</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -26940,7 +26947,7 @@
       </c>
       <c r="I46" s="163">
         <f>A!M35</f>
-        <v>1.25411506840063E-4</v>
+        <v>1.2541161004577301E-4</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -27014,7 +27021,7 @@
       </c>
       <c r="I48" s="246">
         <f>A!M37</f>
-        <v>1.25411506840063E-4</v>
+        <v>1.2541161004577301E-4</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -27088,7 +27095,7 @@
       </c>
       <c r="I50" s="163">
         <f>A!M39</f>
-        <v>1.6783451392009399E-4</v>
+        <v>1.6783452403930699E-4</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="14" thickBot="1">
@@ -27161,11 +27168,11 @@
       <c r="B54" s="166"/>
       <c r="C54" s="167"/>
       <c r="D54" s="168"/>
-      <c r="E54" s="362" t="s">
+      <c r="E54" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="F54" s="363"/>
-      <c r="G54" s="364"/>
+      <c r="F54" s="367"/>
+      <c r="G54" s="368"/>
       <c r="H54" s="169" t="s">
         <v>97</v>
       </c>
@@ -27323,7 +27330,7 @@
       </c>
       <c r="I59" s="257">
         <f>A!E49</f>
-        <v>473.17510592572899</v>
+        <v>473.17513981022802</v>
       </c>
       <c r="J59" s="101"/>
     </row>
@@ -27397,7 +27404,7 @@
       </c>
       <c r="I61" s="199">
         <f>A!E51</f>
-        <v>275.51713805122699</v>
+        <v>275.517154662927</v>
       </c>
       <c r="J61" s="101"/>
     </row>
@@ -27471,11 +27478,11 @@
       <c r="B65" s="166"/>
       <c r="C65" s="167"/>
       <c r="D65" s="168"/>
-      <c r="E65" s="362" t="s">
+      <c r="E65" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="F65" s="363"/>
-      <c r="G65" s="364"/>
+      <c r="F65" s="367"/>
+      <c r="G65" s="368"/>
       <c r="H65" s="155"/>
       <c r="I65" s="101"/>
       <c r="J65" s="133"/>
@@ -27662,11 +27669,11 @@
       <c r="B73" s="166"/>
       <c r="C73" s="167"/>
       <c r="D73" s="168"/>
-      <c r="E73" s="362" t="s">
+      <c r="E73" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="F73" s="363"/>
-      <c r="G73" s="364"/>
+      <c r="F73" s="367"/>
+      <c r="G73" s="368"/>
       <c r="H73" s="155"/>
       <c r="I73" s="133"/>
       <c r="J73" s="133"/>
@@ -27859,11 +27866,11 @@
       <c r="B81" s="166"/>
       <c r="C81" s="167"/>
       <c r="D81" s="168"/>
-      <c r="E81" s="362" t="s">
+      <c r="E81" s="366" t="s">
         <v>108</v>
       </c>
-      <c r="F81" s="363"/>
-      <c r="G81" s="364"/>
+      <c r="F81" s="367"/>
+      <c r="G81" s="368"/>
       <c r="H81" s="155"/>
       <c r="I81" s="133"/>
       <c r="J81" s="133"/>

</xml_diff>